<commit_message>
wflow_publish(c("./analysis/*", "code/*"), all = T)
</commit_message>
<xml_diff>
--- a/output/GOres_D62noDIFFRAPA.xlsx
+++ b/output/GOres_D62noDIFFRAPA.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
   <si>
     <t xml:space="preserve">query</t>
   </si>
@@ -56,13 +56,46 @@
     <t xml:space="preserve">parents</t>
   </si>
   <si>
+    <t xml:space="preserve">evidence_codes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">intersection</t>
+  </si>
+  <si>
     <t xml:space="preserve">query_1</t>
   </si>
   <si>
+    <t xml:space="preserve">GO:0007186</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GO:BP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">G protein-coupled receptor signaling pathway</t>
+  </si>
+  <si>
     <t xml:space="preserve">GO:0007165</t>
   </si>
   <si>
-    <t xml:space="preserve">GO:BP</t>
+    <t xml:space="preserve">IMP,IBA TAS IEA,ISS TAS IEA,IBA IEA,IDA,IDA IPI IGI IBA IEA,TAS,IBA TAS IEA,IMP,IDA TAS IEA,IEA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3925,64123,6004,2775,348,10267,2596,4852,2185,9568,10178</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GO:0007154</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cell communication</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GO:0009987</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IMP TAS NAS,TAS IEA,IBA TAS IEA,ISS TAS IEA,IDA IBA,ISS IBA,IBA,IDA IBA IEA,IEA,TAS IEA,IBA IEA,IDA IBA IEA,IBA IEA,IDA IEA,IDA IMP IGI TAS,IMP,IDA IPI IGI IBA IEA,IMP IBA IEA,IEA,TAS,IDA IMP ISS IBA IEA,IBA,IEA,IDA IMP IEP TAS IEA,ISS,IBA TAS IEA,IDA,ISS IEA,IDA IMP,IEA,IMP ISS IBA TAS IEA,IBA IEA,ISS IEA,IDA ISS IBA TAS NAS IEA,ISS IEA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3925,9077,64123,6004,149111,642938,10581,960,1410,3709,56963,2013,2775,55273,348,79784,10267,1827,1826,2596,3280,3490,8404,1026,4188,4852,23089,1749,5054,4747,2185,5327,2171,9568,10178</t>
   </si>
   <si>
     <t xml:space="preserve">signal transduction</t>
@@ -71,55 +104,40 @@
     <t xml:space="preserve">GO:0007154, GO:0009987, GO:0023052, GO:0050794, GO:0051716</t>
   </si>
   <si>
+    <t xml:space="preserve">IMP TAS NAS,TAS IEA,IBA TAS IEA,ISS TAS IEA,IDA IBA,ISS IBA,IBA,IDA IBA IEA,IEA,TAS IEA,IBA IEA,IDA IBA IEA,IBA IEA,IDA IEA,IDA IMP IGI TAS,IDA IPI IGI IBA IEA,IMP IBA IEA,IEA,TAS,IDA IMP ISS IBA IEA,IBA,IEA,IDA IMP IEP TAS IEA,ISS,IBA TAS IEA,IDA,ISS IEA,IDA IMP,IMP ISS IBA TAS IEA,IBA IEA,IEA,IDA TAS IEA,ISS IEA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3925,9077,64123,6004,149111,642938,10581,960,1410,3709,56963,2013,2775,55273,348,10267,1827,1826,2596,3280,3490,8404,1026,4188,4852,23089,1749,5054,2185,5327,2171,9568,10178</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GO:0032501</t>
+  </si>
+  <si>
+    <t xml:space="preserve">multicellular organismal process</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GO:0008150</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IEA,IBA IEA,TAS,ISS IBA,IEA,IDA IEP,TAS IEA,IEA,ISS IBA IEA,IEA,IDA IMP ISS IEA,TAS,ISS IEA,IEP ISS TAS IEA,IEA,IDA IMP IGI ISS IBA TAS IEA,IMP,IDA,IEA,IDA ISS IBA TAS IEA,IBA IEA,IEA,IEA,IEP ISS IBA TAS IEA,IEA,ISS IEA,ISS IEA,IEP ISS IBA TAS IEA,ISS TAS IEA,IDA IMP IGI IEP IBA TAS NAS IC,IEA,IDA IMP ISS IEA,ISS TAS NAS IEA,IDA IBA,IMP ISS IEA,IMP,IBA TAS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">64856,3925,6004,642938,4004,960,1410,771,57611,56963,2013,2775,55273,361,1995,348,79784,10267,1827,1826,2596,5947,4071,3280,3490,1026,4188,4852,1749,5054,4747,2185,5327,11075,2171,5358,10178</t>
+  </si>
+  <si>
     <t xml:space="preserve">GO:0023052</t>
   </si>
   <si>
     <t xml:space="preserve">signaling</t>
   </si>
   <si>
-    <t xml:space="preserve">GO:0008150</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GO:0051716</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cellular response to stimulus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GO:0009987, GO:0050896</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GO:0007154</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cell communication</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GO:0009987</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GO:0009719</t>
-  </si>
-  <si>
-    <t xml:space="preserve">response to endogenous stimulus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GO:0050896</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GO:0007186</t>
-  </si>
-  <si>
-    <t xml:space="preserve">G protein-coupled receptor signaling pathway</t>
-  </si>
-  <si>
-    <t xml:space="preserve">response to stimulus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GO:0032501</t>
-  </si>
-  <si>
-    <t xml:space="preserve">multicellular organismal process</t>
+    <t xml:space="preserve">GO:0050789</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IMP TAS NAS,TAS IEA,IBA TAS IEA,ISS TAS IEA,IDA IBA,ISS IBA,IBA,IDA IBA IEA,IEA,TAS IEA,IBA IEA,IDA IBA IEA,IBA IEA,IDA IEA,IDA IMP IGI TAS,IDA IPI IGI IBA IEA,IMP IBA IEA,IEA,TAS,IDA IMP ISS IBA IEA,IBA,IEA,IDA IMP IEP TAS IEA,ISS,IBA TAS IEA,IDA,ISS IEA,IDA IMP,IEA,IMP ISS IBA TAS IEA,IBA IEA,ISS IEA,IDA ISS IBA TAS NAS IEA,ISS IEA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3925,9077,64123,6004,149111,642938,10581,960,1410,3709,56963,2013,2775,55273,348,10267,1827,1826,2596,3280,3490,8404,1026,4188,4852,23089,1749,5054,4747,2185,5327,2171,9568,10178</t>
   </si>
   <si>
     <t xml:space="preserve">GO:0071944</t>
@@ -134,6 +152,12 @@
     <t xml:space="preserve">GO:0110165</t>
   </si>
   <si>
+    <t xml:space="preserve">HDA IEA,IBA IEA,ISS IBA IEA,TAS,ISS IEA,IBA TAS IEA,IDA IBA TAS NAS IEA,IEA,IDA IBA IEA,IBA TAS IEA,IEA,IBA IEA,IDA ISS IBA IEA,IDA IBA TAS IEA,IDA IBA IEA,ISS TAS,IDA ISS IBA TAS IEA,IDA HDA TAS,IDA TAS,ISS IBA TAS IEA,IDA IBA TAS IEA,IDA,HDA,IEA,TAS,IDA HDA TAS NAS,ISS IBA IEA,TAS,IDA IPI IBA TAS IEA,IDA,ISS IEA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">64856,9077,64123,6004,149111,10581,960,1410,3709,771,57611,56963,2013,2775,55273,11031,361,348,10267,1826,2596,4071,3490,8404,25798,5054,2185,2171,9568,5358,10178</t>
+  </si>
+  <si>
     <t xml:space="preserve">HPA:0400241</t>
   </si>
   <si>
@@ -144,6 +168,24 @@
   </si>
   <si>
     <t xml:space="preserve">HPA:0400000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enhanced,Enhanced,Enhanced,Enhanced,Enhanced,Enhanced,Enhanced</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3925,960,771,2775,1995,4747,9568</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HPA:0400242</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rectum; peripheral nerve/ganglion[≥Medium]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enhanced,Enhanced,Enhanced,Enhanced,Enhanced,Enhanced</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3925,960,771,2775,1995,9568</t>
   </si>
 </sst>
 </file>
@@ -518,445 +560,411 @@
       <c r="N1" t="s">
         <v>13</v>
       </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B2" t="b">
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>0.00306102355956659</v>
+        <v>0.00541672960494956</v>
       </c>
       <c r="D2" t="n">
-        <v>3294</v>
+        <v>341</v>
       </c>
       <c r="E2" t="n">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="F2" t="n">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="G2" t="n">
-        <v>0.64</v>
+        <v>0.203703703703704</v>
       </c>
       <c r="H2" t="n">
-        <v>0.00971463266545234</v>
+        <v>0.032258064516129</v>
       </c>
       <c r="I2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="J2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="K2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="L2" t="n">
-        <v>12068</v>
+        <v>13136</v>
       </c>
       <c r="M2" t="n">
-        <v>3065</v>
+        <v>2809</v>
       </c>
       <c r="N2" t="s">
-        <v>18</v>
+        <v>20</v>
+      </c>
+      <c r="O2" t="s">
+        <v>21</v>
+      </c>
+      <c r="P2" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B3" t="b">
         <v>1</v>
       </c>
       <c r="C3" t="n">
-        <v>0.00657148982916446</v>
+        <v>0.00654783311107867</v>
       </c>
       <c r="D3" t="n">
-        <v>3601</v>
+        <v>3946</v>
       </c>
       <c r="E3" t="n">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="F3" t="n">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G3" t="n">
-        <v>0.66</v>
+        <v>0.648148148148148</v>
       </c>
       <c r="H3" t="n">
-        <v>0.00916412107747848</v>
+        <v>0.00886974151039027</v>
       </c>
       <c r="I3" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="J3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="K3" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="L3" t="n">
-        <v>12068</v>
+        <v>13136</v>
       </c>
       <c r="M3" t="n">
-        <v>7648</v>
+        <v>2781</v>
       </c>
       <c r="N3" t="s">
-        <v>21</v>
+        <v>25</v>
+      </c>
+      <c r="O3" t="s">
+        <v>26</v>
+      </c>
+      <c r="P3" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B4" t="b">
         <v>1</v>
       </c>
       <c r="C4" t="n">
-        <v>0.0082213354005545</v>
+        <v>0.00807321228445205</v>
       </c>
       <c r="D4" t="n">
-        <v>4294</v>
+        <v>3561</v>
       </c>
       <c r="E4" t="n">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="F4" t="n">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="G4" t="n">
-        <v>0.72</v>
+        <v>0.611111111111111</v>
       </c>
       <c r="H4" t="n">
-        <v>0.00838379133674895</v>
+        <v>0.0092670598146588</v>
       </c>
       <c r="I4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="J4" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="K4" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="L4" t="n">
-        <v>12068</v>
+        <v>13136</v>
       </c>
       <c r="M4" t="n">
-        <v>16064</v>
+        <v>2792</v>
       </c>
       <c r="N4" t="s">
-        <v>24</v>
+        <v>29</v>
+      </c>
+      <c r="O4" t="s">
+        <v>30</v>
+      </c>
+      <c r="P4" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B5" t="b">
         <v>1</v>
       </c>
       <c r="C5" t="n">
-        <v>0.00897051046431474</v>
+        <v>0.0124023907665696</v>
       </c>
       <c r="D5" t="n">
-        <v>3644</v>
+        <v>4480</v>
       </c>
       <c r="E5" t="n">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="F5" t="n">
+        <v>37</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0.685185185185185</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0.00825892857142857</v>
+      </c>
+      <c r="I5" t="s">
+        <v>32</v>
+      </c>
+      <c r="J5" t="s">
+        <v>18</v>
+      </c>
+      <c r="K5" t="s">
         <v>33</v>
       </c>
-      <c r="G5" t="n">
-        <v>0.66</v>
-      </c>
-      <c r="H5" t="n">
-        <v>0.00905598243688255</v>
-      </c>
-      <c r="I5" t="s">
-        <v>25</v>
-      </c>
-      <c r="J5" t="s">
-        <v>16</v>
-      </c>
-      <c r="K5" t="s">
-        <v>26</v>
-      </c>
       <c r="L5" t="n">
-        <v>12068</v>
+        <v>13136</v>
       </c>
       <c r="M5" t="n">
-        <v>3054</v>
+        <v>8031</v>
       </c>
       <c r="N5" t="s">
-        <v>27</v>
+        <v>34</v>
+      </c>
+      <c r="O5" t="s">
+        <v>35</v>
+      </c>
+      <c r="P5" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B6" t="b">
         <v>1</v>
       </c>
       <c r="C6" t="n">
-        <v>0.0115111491610182</v>
+        <v>0.0165520440519194</v>
       </c>
       <c r="D6" t="n">
-        <v>993</v>
+        <v>3870</v>
       </c>
       <c r="E6" t="n">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="F6" t="n">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="G6" t="n">
-        <v>0.34</v>
+        <v>0.62962962962963</v>
       </c>
       <c r="H6" t="n">
-        <v>0.0171198388721047</v>
+        <v>0.00878552971576227</v>
       </c>
       <c r="I6" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="J6" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="K6" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="L6" t="n">
-        <v>12068</v>
+        <v>13136</v>
       </c>
       <c r="M6" t="n">
-        <v>4067</v>
+        <v>7002</v>
       </c>
       <c r="N6" t="s">
-        <v>30</v>
+        <v>39</v>
+      </c>
+      <c r="O6" t="s">
+        <v>40</v>
+      </c>
+      <c r="P6" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B7" t="b">
         <v>1</v>
       </c>
       <c r="C7" t="n">
-        <v>0.0251513245072741</v>
+        <v>0.0152076867225957</v>
       </c>
       <c r="D7" t="n">
-        <v>314</v>
+        <v>3251</v>
       </c>
       <c r="E7" t="n">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="F7" t="n">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="G7" t="n">
-        <v>0.2</v>
+        <v>0.574074074074074</v>
       </c>
       <c r="H7" t="n">
-        <v>0.0318471337579618</v>
+        <v>0.00953552752999077</v>
       </c>
       <c r="I7" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="J7" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="K7" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="L7" t="n">
-        <v>12068</v>
+        <v>13136</v>
       </c>
       <c r="M7" t="n">
-        <v>3084</v>
+        <v>2801</v>
       </c>
       <c r="N7" t="s">
-        <v>15</v>
+        <v>45</v>
+      </c>
+      <c r="O7" t="s">
+        <v>46</v>
+      </c>
+      <c r="P7" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B8" t="b">
         <v>1</v>
       </c>
       <c r="C8" t="n">
-        <v>0.0262794363351145</v>
+        <v>0.00589799705776251</v>
       </c>
       <c r="D8" t="n">
-        <v>4956</v>
+        <v>215</v>
       </c>
       <c r="E8" t="n">
+        <v>54</v>
+      </c>
+      <c r="F8" t="n">
+        <v>7</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0.12962962962963</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0.0325581395348837</v>
+      </c>
+      <c r="I8" t="s">
+        <v>48</v>
+      </c>
+      <c r="J8" t="s">
+        <v>49</v>
+      </c>
+      <c r="K8" t="s">
         <v>50</v>
       </c>
-      <c r="F8" t="n">
-        <v>38</v>
-      </c>
-      <c r="G8" t="n">
-        <v>0.76</v>
-      </c>
-      <c r="H8" t="n">
-        <v>0.00766747376916868</v>
-      </c>
-      <c r="I8" t="s">
-        <v>30</v>
-      </c>
-      <c r="J8" t="s">
-        <v>16</v>
-      </c>
-      <c r="K8" t="s">
-        <v>33</v>
-      </c>
       <c r="L8" t="n">
-        <v>12068</v>
+        <v>13136</v>
       </c>
       <c r="M8" t="n">
-        <v>15410</v>
+        <v>571</v>
       </c>
       <c r="N8" t="s">
-        <v>21</v>
+        <v>51</v>
+      </c>
+      <c r="O8" t="s">
+        <v>52</v>
+      </c>
+      <c r="P8" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B9" t="b">
         <v>1</v>
       </c>
       <c r="C9" t="n">
-        <v>0.0368372958388359</v>
+        <v>0.0109962724827968</v>
       </c>
       <c r="D9" t="n">
-        <v>4068</v>
+        <v>161</v>
       </c>
       <c r="E9" t="n">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="F9" t="n">
-        <v>34</v>
+        <v>6</v>
       </c>
       <c r="G9" t="n">
-        <v>0.68</v>
+        <v>0.111111111111111</v>
       </c>
       <c r="H9" t="n">
-        <v>0.00835791543756145</v>
+        <v>0.0372670807453416</v>
       </c>
       <c r="I9" t="s">
-        <v>34</v>
+        <v>54</v>
       </c>
       <c r="J9" t="s">
-        <v>16</v>
+        <v>49</v>
       </c>
       <c r="K9" t="s">
-        <v>35</v>
+        <v>55</v>
       </c>
       <c r="L9" t="n">
-        <v>12068</v>
+        <v>13136</v>
       </c>
       <c r="M9" t="n">
-        <v>8803</v>
+        <v>572</v>
       </c>
       <c r="N9" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" t="b">
-        <v>1</v>
-      </c>
-      <c r="C10" t="n">
-        <v>0.0371066161268442</v>
-      </c>
-      <c r="D10" t="n">
-        <v>3029</v>
-      </c>
-      <c r="E10" t="n">
-        <v>50</v>
-      </c>
-      <c r="F10" t="n">
-        <v>29</v>
-      </c>
-      <c r="G10" t="n">
-        <v>0.58</v>
-      </c>
-      <c r="H10" t="n">
-        <v>0.00957411687025421</v>
-      </c>
-      <c r="I10" t="s">
-        <v>36</v>
-      </c>
-      <c r="J10" t="s">
-        <v>37</v>
-      </c>
-      <c r="K10" t="s">
-        <v>38</v>
-      </c>
-      <c r="L10" t="n">
-        <v>12068</v>
-      </c>
-      <c r="M10" t="n">
-        <v>3128</v>
-      </c>
-      <c r="N10" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" t="b">
-        <v>1</v>
-      </c>
-      <c r="C11" t="n">
-        <v>0.0286976984703445</v>
-      </c>
-      <c r="D11" t="n">
-        <v>192</v>
-      </c>
-      <c r="E11" t="n">
-        <v>50</v>
-      </c>
-      <c r="F11" t="n">
-        <v>6</v>
-      </c>
-      <c r="G11" t="n">
-        <v>0.12</v>
-      </c>
-      <c r="H11" t="n">
-        <v>0.03125</v>
-      </c>
-      <c r="I11" t="s">
-        <v>40</v>
-      </c>
-      <c r="J11" t="s">
-        <v>41</v>
-      </c>
-      <c r="K11" t="s">
-        <v>42</v>
-      </c>
-      <c r="L11" t="n">
-        <v>12068</v>
-      </c>
-      <c r="M11" t="n">
-        <v>546</v>
-      </c>
-      <c r="N11" t="s">
-        <v>43</v>
+        <v>48</v>
+      </c>
+      <c r="O9" t="s">
+        <v>56</v>
+      </c>
+      <c r="P9" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>